<commit_message>
remove address from db
</commit_message>
<xml_diff>
--- a/api/src/templates/sheetmenu-template.xlsx
+++ b/api/src/templates/sheetmenu-template.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="Business Info" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Dinner Menu" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Lunch Menu" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,48 +13,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>User Name</t>
   </si>
   <si>
+    <t>Test User</t>
+  </si>
+  <si>
     <t>Restaurant Name</t>
   </si>
   <si>
+    <t>Taste of Japan</t>
+  </si>
+  <si>
     <t>Street Address</t>
   </si>
   <si>
+    <t>123 Abby Road</t>
+  </si>
+  <si>
     <t>Apartment, suite, etc</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
+    <t>London</t>
+  </si>
+  <si>
     <t>State/Province</t>
   </si>
   <si>
+    <t>Middlebury</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
+    <t>England</t>
+  </si>
+  <si>
     <t>ZIP/postal code</t>
   </si>
   <si>
+    <t>5V6 8Y7</t>
+  </si>
+  <si>
     <t>Phone number</t>
   </si>
   <si>
+    <t>(416) 123 - 4567</t>
+  </si>
+  <si>
     <t>Restaurant Description (3 sentences max)</t>
   </si>
   <si>
+    <t>Authentic Japanese flavors you won't find anywhere else.
+Recipies handed down for generations. And a serious obession with
+making delicous food.</t>
+  </si>
+  <si>
     <t>Value Prop 1</t>
   </si>
   <si>
+    <t>Fresh Ingredients</t>
+  </si>
+  <si>
     <t>Value Prop 2</t>
   </si>
   <si>
+    <t>Homemade</t>
+  </si>
+  <si>
     <t>Value Prop 3</t>
   </si>
   <si>
-    <t>Header Picture</t>
+    <t>Yummy</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Monday</t>
+  </si>
+  <si>
+    <t>10 - 5pm</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Tuesday</t>
+  </si>
+  <si>
+    <t>11 - 3pm</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Wednesday</t>
+  </si>
+  <si>
+    <t>3 - 9pm</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Thursday</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Friday</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Saturday</t>
+  </si>
+  <si>
+    <t>Hours of Operation: Sunday</t>
+  </si>
+  <si>
+    <t>Hero Picture</t>
   </si>
   <si>
     <t>Name</t>
@@ -66,13 +135,37 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Healthy and delicious</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Crunchy and creamy</t>
+  </si>
+  <si>
+    <t>Item 3</t>
+  </si>
+  <si>
+    <t>Hot and spicy</t>
+  </si>
+  <si>
+    <t>Item 4</t>
+  </si>
+  <si>
+    <t>Savory and flavorful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -80,17 +173,38 @@
     </font>
     <font>
       <b/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <b/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -112,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -120,7 +234,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -128,9 +242,25 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -141,10 +271,43 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1390650" cy="2085975"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -352,720 +515,799 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.57"/>
-    <col customWidth="1" min="2" max="2" width="50.86"/>
-    <col customWidth="1" min="3" max="6" width="14.43"/>
+    <col customWidth="1" min="1" max="1" width="40.71"/>
+    <col customWidth="1" min="2" max="2" width="70.57"/>
+    <col customWidth="1" min="3" max="3" width="47.71"/>
+    <col customWidth="1" min="4" max="4" width="49.29"/>
+    <col customWidth="1" min="5" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" ht="26.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" ht="66.75" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6"/>
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="B15" s="6"/>
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" s="6"/>
+      <c r="A16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="B17" s="6"/>
+      <c r="A17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="6"/>
+      <c r="A18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="6"/>
+      <c r="A19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="6"/>
+      <c r="A20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" ht="164.25" customHeight="1">
+      <c r="A21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="9"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="6"/>
+      <c r="B22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="6"/>
+      <c r="B23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="6"/>
+      <c r="B24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="6"/>
+      <c r="B25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="6"/>
+      <c r="B26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="6"/>
+      <c r="B27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="6"/>
+      <c r="B28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="6"/>
+      <c r="B29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="6"/>
+      <c r="B30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="6"/>
+      <c r="B31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="6"/>
+      <c r="B32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="6"/>
+      <c r="B33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="6"/>
+      <c r="B34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="6"/>
+      <c r="B35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="6"/>
+      <c r="B36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="6"/>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="6"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="B39" s="6"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="B40" s="6"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="6"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="6"/>
+      <c r="B42" s="10"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="6"/>
+      <c r="B43" s="10"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="6"/>
+      <c r="B44" s="10"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="6"/>
+      <c r="B45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="6"/>
+      <c r="B46" s="10"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="6"/>
+      <c r="B47" s="10"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="6"/>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="6"/>
+      <c r="B49" s="10"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="6"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="6"/>
+      <c r="B51" s="10"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="6"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="6"/>
+      <c r="B53" s="10"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="6"/>
+      <c r="B54" s="10"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="6"/>
+      <c r="B55" s="10"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="6"/>
+      <c r="B56" s="10"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="6"/>
+      <c r="B57" s="10"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="B58" s="6"/>
+      <c r="B58" s="10"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="6"/>
+      <c r="B59" s="10"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="B60" s="6"/>
+      <c r="B60" s="10"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="6"/>
+      <c r="B61" s="10"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="6"/>
+      <c r="B62" s="10"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="6"/>
+      <c r="B63" s="10"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="6"/>
+      <c r="B64" s="10"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="6"/>
+      <c r="B65" s="10"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="6"/>
+      <c r="B66" s="10"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="6"/>
+      <c r="B67" s="10"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="6"/>
+      <c r="B68" s="10"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="B69" s="6"/>
+      <c r="B69" s="10"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="B70" s="6"/>
+      <c r="B70" s="10"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="6"/>
+      <c r="B71" s="10"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="6"/>
+      <c r="B72" s="10"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="6"/>
+      <c r="B73" s="10"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="6"/>
+      <c r="B74" s="10"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="B75" s="6"/>
+      <c r="B75" s="10"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="B76" s="6"/>
+      <c r="B76" s="10"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="B77" s="6"/>
+      <c r="B77" s="10"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="B78" s="6"/>
+      <c r="B78" s="10"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="B79" s="6"/>
+      <c r="B79" s="10"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="B80" s="6"/>
+      <c r="B80" s="10"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="B81" s="6"/>
+      <c r="B81" s="10"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="B82" s="6"/>
+      <c r="B82" s="10"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="B83" s="6"/>
+      <c r="B83" s="10"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="B84" s="6"/>
+      <c r="B84" s="10"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="B85" s="6"/>
+      <c r="B85" s="10"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="B86" s="6"/>
+      <c r="B86" s="10"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="B87" s="6"/>
+      <c r="B87" s="10"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="B88" s="6"/>
+      <c r="B88" s="10"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="B89" s="6"/>
+      <c r="B89" s="10"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="B90" s="6"/>
+      <c r="B90" s="10"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="B91" s="6"/>
+      <c r="B91" s="10"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="B92" s="6"/>
+      <c r="B92" s="10"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="B93" s="6"/>
+      <c r="B93" s="10"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="B94" s="6"/>
+      <c r="B94" s="10"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="B95" s="6"/>
+      <c r="B95" s="10"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="B96" s="6"/>
+      <c r="B96" s="10"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="B97" s="6"/>
+      <c r="B97" s="10"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="B98" s="6"/>
+      <c r="B98" s="10"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="B99" s="6"/>
+      <c r="B99" s="10"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="B100" s="6"/>
+      <c r="B100" s="10"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="B101" s="6"/>
+      <c r="B101" s="10"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="B102" s="6"/>
+      <c r="B102" s="10"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="B103" s="6"/>
+      <c r="B103" s="10"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="B104" s="6"/>
+      <c r="B104" s="10"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="B105" s="6"/>
+      <c r="B105" s="10"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="B106" s="6"/>
+      <c r="B106" s="10"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="B107" s="6"/>
+      <c r="B107" s="10"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="B108" s="6"/>
+      <c r="B108" s="10"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="B109" s="6"/>
+      <c r="B109" s="10"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="B110" s="6"/>
+      <c r="B110" s="10"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="B111" s="6"/>
+      <c r="B111" s="10"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="B112" s="6"/>
+      <c r="B112" s="10"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="B113" s="6"/>
+      <c r="B113" s="10"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="B114" s="6"/>
+      <c r="B114" s="10"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="B115" s="6"/>
+      <c r="B115" s="10"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="B116" s="6"/>
+      <c r="B116" s="10"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="B117" s="6"/>
+      <c r="B117" s="10"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="B118" s="6"/>
+      <c r="B118" s="10"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="B119" s="6"/>
+      <c r="B119" s="10"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="B120" s="6"/>
+      <c r="B120" s="10"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="B121" s="6"/>
+      <c r="B121" s="10"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="B122" s="6"/>
+      <c r="B122" s="10"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="B123" s="6"/>
+      <c r="B123" s="10"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="B124" s="6"/>
+      <c r="B124" s="10"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="B125" s="6"/>
+      <c r="B125" s="10"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="B126" s="6"/>
+      <c r="B126" s="10"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="B127" s="6"/>
+      <c r="B127" s="10"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="B128" s="6"/>
+      <c r="B128" s="10"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="B129" s="6"/>
+      <c r="B129" s="10"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="B130" s="6"/>
+      <c r="B130" s="10"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="B131" s="6"/>
+      <c r="B131" s="10"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="B132" s="6"/>
+      <c r="B132" s="10"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="B133" s="6"/>
+      <c r="B133" s="10"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="B134" s="6"/>
+      <c r="B134" s="10"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="B135" s="6"/>
+      <c r="B135" s="10"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="B136" s="6"/>
+      <c r="B136" s="10"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="B137" s="6"/>
+      <c r="B137" s="10"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="B138" s="6"/>
+      <c r="B138" s="10"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="B139" s="6"/>
+      <c r="B139" s="10"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="B140" s="6"/>
+      <c r="B140" s="10"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="B141" s="6"/>
+      <c r="B141" s="10"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="B142" s="6"/>
+      <c r="B142" s="10"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="B143" s="6"/>
+      <c r="B143" s="10"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="B144" s="6"/>
+      <c r="B144" s="10"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="B145" s="6"/>
+      <c r="B145" s="10"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="B146" s="6"/>
+      <c r="B146" s="10"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="B147" s="6"/>
+      <c r="B147" s="10"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="B148" s="6"/>
+      <c r="B148" s="10"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="B149" s="6"/>
+      <c r="B149" s="10"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="B150" s="6"/>
+      <c r="B150" s="10"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="B151" s="6"/>
+      <c r="B151" s="10"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="B152" s="6"/>
+      <c r="B152" s="10"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="B153" s="6"/>
+      <c r="B153" s="10"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="B154" s="6"/>
+      <c r="B154" s="10"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="B155" s="6"/>
+      <c r="B155" s="10"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="B156" s="6"/>
+      <c r="B156" s="10"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="B157" s="6"/>
+      <c r="B157" s="10"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="B158" s="6"/>
+      <c r="B158" s="10"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="B159" s="6"/>
+      <c r="B159" s="10"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="B160" s="6"/>
+      <c r="B160" s="10"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="B161" s="6"/>
+      <c r="B161" s="10"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="B162" s="6"/>
+      <c r="B162" s="10"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="B163" s="6"/>
+      <c r="B163" s="10"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="B164" s="6"/>
+      <c r="B164" s="10"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="B165" s="6"/>
+      <c r="B165" s="10"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="B166" s="6"/>
+      <c r="B166" s="10"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="B167" s="6"/>
+      <c r="B167" s="10"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="B168" s="6"/>
+      <c r="B168" s="10"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="B169" s="6"/>
+      <c r="B169" s="10"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="B170" s="6"/>
+      <c r="B170" s="10"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="B171" s="6"/>
+      <c r="B171" s="10"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="B172" s="6"/>
+      <c r="B172" s="10"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="B173" s="6"/>
+      <c r="B173" s="10"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="B174" s="6"/>
+      <c r="B174" s="10"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="B175" s="6"/>
+      <c r="B175" s="10"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="B176" s="6"/>
+      <c r="B176" s="10"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="B177" s="6"/>
+      <c r="B177" s="10"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="B178" s="6"/>
+      <c r="B178" s="10"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="B179" s="6"/>
+      <c r="B179" s="10"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="B180" s="6"/>
+      <c r="B180" s="10"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="B181" s="6"/>
+      <c r="B181" s="10"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="B182" s="6"/>
+      <c r="B182" s="10"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="B183" s="6"/>
+      <c r="B183" s="10"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="B184" s="6"/>
+      <c r="B184" s="10"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="B185" s="6"/>
+      <c r="B185" s="10"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="B186" s="6"/>
+      <c r="B186" s="10"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="B187" s="6"/>
+      <c r="B187" s="10"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="6"/>
+      <c r="B188" s="10"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="B189" s="6"/>
+      <c r="B189" s="10"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="B190" s="6"/>
+      <c r="B190" s="10"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="B191" s="6"/>
+      <c r="B191" s="10"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="B192" s="6"/>
+      <c r="B192" s="10"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="B193" s="6"/>
+      <c r="B193" s="10"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="B194" s="6"/>
+      <c r="B194" s="10"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="B195" s="6"/>
+      <c r="B195" s="10"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="B196" s="6"/>
+      <c r="B196" s="10"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="B197" s="6"/>
+      <c r="B197" s="10"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="B198" s="6"/>
+      <c r="B198" s="10"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="B199" s="6"/>
+      <c r="B199" s="10"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="B200" s="6"/>
+      <c r="B200" s="10"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="B201" s="6"/>
+      <c r="B201" s="10"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="B202" s="6"/>
+      <c r="B202" s="10"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="B203" s="6"/>
+      <c r="B203" s="10"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="B204" s="6"/>
+      <c r="B204" s="10"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="B205" s="6"/>
+      <c r="B205" s="10"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="B206" s="6"/>
+      <c r="B206" s="10"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="B207" s="6"/>
+      <c r="B207" s="10"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="B208" s="6"/>
+      <c r="B208" s="10"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="B209" s="6"/>
+      <c r="B209" s="10"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="B210" s="6"/>
+      <c r="B210" s="10"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="B211" s="6"/>
+      <c r="B211" s="10"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="B212" s="6"/>
+      <c r="B212" s="10"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="B213" s="6"/>
+      <c r="B213" s="10"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="B214" s="6"/>
+      <c r="B214" s="10"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="B215" s="6"/>
+      <c r="B215" s="10"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="B216" s="6"/>
+      <c r="B216" s="10"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="B217" s="6"/>
+      <c r="B217" s="10"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="B218" s="6"/>
+      <c r="B218" s="10"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="B219" s="6"/>
+      <c r="B219" s="10"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="B220" s="6"/>
-    </row>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
+      <c r="B220" s="10"/>
+    </row>
+    <row r="221" ht="15.75" customHeight="1">
+      <c r="B221" s="10"/>
+    </row>
+    <row r="222" ht="15.75" customHeight="1">
+      <c r="B222" s="10"/>
+    </row>
+    <row r="223" ht="15.75" customHeight="1">
+      <c r="B223" s="10"/>
+    </row>
+    <row r="224" ht="15.75" customHeight="1">
+      <c r="B224" s="10"/>
+    </row>
+    <row r="225" ht="15.75" customHeight="1">
+      <c r="B225" s="10"/>
+    </row>
+    <row r="226" ht="15.75" customHeight="1">
+      <c r="B226" s="10"/>
+    </row>
+    <row r="227" ht="15.75" customHeight="1">
+      <c r="B227" s="10"/>
+    </row>
     <row r="228" ht="15.75" customHeight="1"/>
     <row r="229" ht="15.75" customHeight="1"/>
     <row r="230" ht="15.75" customHeight="1"/>
@@ -1839,6 +2081,13 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1860,23 +2109,63 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1"/>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
+      <c r="A1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -2875,4 +3164,80 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="21.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="12">
+        <v>9.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>